<commit_message>
camacho - subindo aula de tabbar
</commit_message>
<xml_diff>
--- a/2des/frequencia.xlsx
+++ b/2des/frequencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2023\2des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49C5A72-F472-4F79-BE84-0C536BE1FE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DFDCF1-E62A-48D2-8C98-7E0CC27D0B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2269" uniqueCount="41">
   <si>
     <t>Andre Fernandes Izidro</t>
   </si>
@@ -580,7 +580,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="BJ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BZ30" sqref="BZ30"/>
+      <selection pane="bottomRight" activeCell="CA31" sqref="CA31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1333,9 @@
       <c r="BZ3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="CA3" s="4"/>
+      <c r="CA3" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB3" s="4"/>
       <c r="CC3" s="4"/>
       <c r="CD3" s="4"/>
@@ -1594,7 +1596,9 @@
       <c r="BZ4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="CA4" s="4"/>
+      <c r="CA4" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB4" s="4"/>
       <c r="CC4" s="4"/>
       <c r="CD4" s="4"/>
@@ -2219,7 +2223,9 @@
       <c r="BZ7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="CA7" s="4"/>
+      <c r="CA7" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB7" s="4"/>
       <c r="CC7" s="4"/>
       <c r="CD7" s="4"/>
@@ -2480,7 +2486,9 @@
       <c r="BZ8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA8" s="4"/>
+      <c r="CA8" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB8" s="4"/>
       <c r="CC8" s="4"/>
       <c r="CD8" s="4"/>
@@ -2743,7 +2751,9 @@
       <c r="BZ9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA9" s="4"/>
+      <c r="CA9" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB9" s="4"/>
       <c r="CC9" s="4"/>
       <c r="CD9" s="4"/>
@@ -3006,7 +3016,9 @@
       <c r="BZ10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="CA10" s="4"/>
+      <c r="CA10" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB10" s="4"/>
       <c r="CC10" s="4"/>
       <c r="CD10" s="4"/>
@@ -3269,7 +3281,9 @@
       <c r="BZ11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA11" s="4"/>
+      <c r="CA11" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB11" s="4"/>
       <c r="CC11" s="4"/>
       <c r="CD11" s="4"/>
@@ -3532,7 +3546,9 @@
       <c r="BZ12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="CA12" s="4"/>
+      <c r="CA12" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB12" s="4"/>
       <c r="CC12" s="4"/>
       <c r="CD12" s="4"/>
@@ -3795,7 +3811,9 @@
       <c r="BZ13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA13" s="4"/>
+      <c r="CA13" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB13" s="4"/>
       <c r="CC13" s="4"/>
       <c r="CD13" s="4"/>
@@ -4058,7 +4076,9 @@
       <c r="BZ14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA14" s="4"/>
+      <c r="CA14" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB14" s="4"/>
       <c r="CC14" s="4"/>
       <c r="CD14" s="4"/>
@@ -4321,7 +4341,9 @@
       <c r="BZ15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA15" s="4"/>
+      <c r="CA15" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="CB15" s="4"/>
       <c r="CC15" s="4"/>
       <c r="CD15" s="4"/>
@@ -4584,7 +4606,9 @@
       <c r="BZ16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA16" s="4"/>
+      <c r="CA16" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB16" s="4"/>
       <c r="CC16" s="4"/>
       <c r="CD16" s="4"/>
@@ -4847,7 +4871,9 @@
       <c r="BZ17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA17" s="4"/>
+      <c r="CA17" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB17" s="4"/>
       <c r="CC17" s="4"/>
       <c r="CD17" s="4"/>
@@ -5110,7 +5136,9 @@
       <c r="BZ18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA18" s="4"/>
+      <c r="CA18" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB18" s="4"/>
       <c r="CC18" s="4"/>
       <c r="CD18" s="4"/>
@@ -5373,7 +5401,9 @@
       <c r="BZ19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA19" s="4"/>
+      <c r="CA19" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB19" s="4"/>
       <c r="CC19" s="4"/>
       <c r="CD19" s="4"/>
@@ -5636,7 +5666,9 @@
       <c r="BZ20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA20" s="4"/>
+      <c r="CA20" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB20" s="4"/>
       <c r="CC20" s="4"/>
       <c r="CD20" s="4"/>
@@ -5899,7 +5931,9 @@
       <c r="BZ21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA21" s="4"/>
+      <c r="CA21" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB21" s="4"/>
       <c r="CC21" s="4"/>
       <c r="CD21" s="4"/>
@@ -6162,7 +6196,9 @@
       <c r="BZ22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA22" s="4"/>
+      <c r="CA22" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB22" s="4"/>
       <c r="CC22" s="4"/>
       <c r="CD22" s="4"/>
@@ -6425,7 +6461,9 @@
       <c r="BZ23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA23" s="4"/>
+      <c r="CA23" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB23" s="4"/>
       <c r="CC23" s="4"/>
       <c r="CD23" s="4"/>
@@ -6688,7 +6726,9 @@
       <c r="BZ24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="CA24" s="4"/>
+      <c r="CA24" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB24" s="4"/>
       <c r="CC24" s="4"/>
       <c r="CD24" s="4"/>
@@ -6951,7 +6991,9 @@
       <c r="BZ25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA25" s="4"/>
+      <c r="CA25" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB25" s="4"/>
       <c r="CC25" s="4"/>
       <c r="CD25" s="4"/>
@@ -7214,7 +7256,9 @@
       <c r="BZ26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA26" s="4"/>
+      <c r="CA26" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB26" s="4"/>
       <c r="CC26" s="4"/>
       <c r="CD26" s="4"/>
@@ -7477,7 +7521,9 @@
       <c r="BZ27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA27" s="4"/>
+      <c r="CA27" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="CB27" s="4"/>
       <c r="CC27" s="4"/>
       <c r="CD27" s="4"/>
@@ -7740,7 +7786,9 @@
       <c r="BZ28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA28" s="4"/>
+      <c r="CA28" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB28" s="4"/>
       <c r="CC28" s="4"/>
       <c r="CD28" s="4"/>
@@ -8003,7 +8051,9 @@
       <c r="BZ29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA29" s="4"/>
+      <c r="CA29" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB29" s="4"/>
       <c r="CC29" s="4"/>
       <c r="CD29" s="4"/>
@@ -8266,7 +8316,9 @@
       <c r="BZ30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA30" s="4"/>
+      <c r="CA30" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB30" s="4"/>
       <c r="CC30" s="4"/>
       <c r="CD30" s="4"/>
@@ -8529,7 +8581,9 @@
       <c r="BZ31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="CA31" s="4"/>
+      <c r="CA31" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="CB31" s="4"/>
       <c r="CC31" s="4"/>
       <c r="CD31" s="4"/>

</xml_diff>